<commit_message>
Added review and retrospective for this sprint
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/Scrum.xlsx
+++ b/Documentation/Scrum/Scrum.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\SDJ_Course\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\SDJ_Course\Documentation\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="88">
   <si>
     <t>Actual remaining hours</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t>Junit test for proxy design pattern</t>
-  </si>
-  <si>
-    <t>Not started</t>
   </si>
   <si>
     <t>Fix displaying trips in date interval in GUI</t>
@@ -1793,7 +1790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1948,7 +1945,7 @@
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="5">
         <v>18</v>
@@ -2093,7 +2090,7 @@
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="5">
         <v>2</v>
@@ -2431,7 +2428,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3258,8 +3255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3323,7 +3320,7 @@
         <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -3340,7 +3337,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -3360,10 +3357,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -3380,16 +3377,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3400,7 +3397,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Finished mvc doc and filled table in scrum file.
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/Scrum.xlsx
+++ b/Documentation/Scrum/Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -589,13 +589,13 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1790,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1975,12 +1975,14 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6">
+        <v>9</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2138,15 +2140,15 @@
       </c>
       <c r="G16" s="5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3255,7 +3257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final documennt with scrum and abstract
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/Scrum.xlsx
+++ b/Documentation/Scrum/Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,11 @@
     <sheet name="26.04" sheetId="9" r:id="rId5"/>
     <sheet name="28.04" sheetId="10" r:id="rId6"/>
     <sheet name="01.05" sheetId="11" r:id="rId7"/>
+    <sheet name="03.05" sheetId="12" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'01.05'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'03.05'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'22.04'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'24.04'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'26.04'!$A$1:$F$1</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="90">
   <si>
     <t>Actual remaining hours</t>
   </si>
@@ -301,6 +303,12 @@
   </si>
   <si>
     <t>Martin, Stela</t>
+  </si>
+  <si>
+    <t>Final touches</t>
+  </si>
+  <si>
+    <t>Final documentation</t>
   </si>
 </sst>
 </file>
@@ -1790,7 +1798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -3414,4 +3422,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>